<commit_message>
Unsaved changed to Excel
</commit_message>
<xml_diff>
--- a/reporting/chart_source.xlsx
+++ b/reporting/chart_source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="17560" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="17560" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="fig1_data" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,14 @@
     <sheet name="fig2_chart" sheetId="4" r:id="rId4"/>
     <sheet name="fig3_data" sheetId="5" r:id="rId5"/>
     <sheet name="fig3_chart" sheetId="6" r:id="rId6"/>
+    <sheet name="fig4_data" sheetId="7" r:id="rId7"/>
+    <sheet name="fig4_chart" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="mv_ev" localSheetId="2">fig2_data!$A$1:$B$52</definedName>
     <definedName name="pop_ev" localSheetId="0">fig1_data!$A$1:$C$52</definedName>
     <definedName name="pop_ev" localSheetId="2">fig2_data!#REF!</definedName>
+    <definedName name="solution" localSheetId="6">fig4_data!$A$1:$C$27</definedName>
     <definedName name="time_series" localSheetId="4">fig3_data!$A$1:$C$40</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -48,7 +51,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="time_series.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="solution.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="the_bends:Users:adamrneary:Developer:election-results:analysis:solution.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="time_series.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="the_bends:Users:adamrneary:Developer:election-results:analysis:time_series.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
@@ -61,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
   <si>
     <t>Alabama</t>
   </si>
@@ -236,6 +248,9 @@
   <si>
     <t>Very Safe State Voters</t>
   </si>
+  <si>
+    <t>Voting Power</t>
+  </si>
 </sst>
 </file>
 
@@ -306,13 +321,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="0"/>
-              <a:t>Voting Power by State Size</a:t>
+              <a:t>Voting Power by State Size (2012)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1081,6 +1096,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2088251656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1088,6 +1113,16 @@
           <c:builtInUnit val="thousands"/>
           <c:dispUnitsLbl>
             <c:layout/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
@@ -1102,6 +1137,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2137323848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
@@ -1177,14 +1222,14 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="0" baseline="0"/>
-              <a:t> Swing vs Safe State</a:t>
+              <a:t> Swing vs Safe State (2012)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="0"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1588,6 +1633,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2137690376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1595,6 +1650,16 @@
           <c:builtInUnit val="thousands"/>
           <c:dispUnitsLbl>
             <c:layout/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
@@ -1650,7 +1715,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2252,6 +2317,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="-2136572664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2264,6 +2339,1624 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000">
+          <a:latin typeface="Concourse C3"/>
+          <a:cs typeface="Concourse C3"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0" i="0" u="none"/>
+              <a:t>National Popular Vote </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0" i="0"/>
+              <a:t>Bill</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0"/>
+              <a:t> Participation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fig4_data!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Voting Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E6B9B8"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="632523"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B9CDE5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="254061"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>fig4_data!$A$2:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>D. C.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>New York</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>New Jersey</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Tennessee</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Kansas</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Vermont</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Wyoming</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fig4_data!$C$2:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>81896.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81464.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70597.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68806.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66663.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63968.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54805.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52031.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51136.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50977.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46410.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46275.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45601.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44214.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42890.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42222.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41650.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>38727.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38601.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35877.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35513.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>34596.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33892.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33203.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30901.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30618.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2131684936"/>
+        <c:axId val="-2130734072"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fig4_data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Electoral Votes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="38000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C0504D"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:marker>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="38000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:xVal>
+            <c:strRef>
+              <c:f>fig4_data!$A$2:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>D. C.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>New York</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>New Jersey</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Tennessee</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Kansas</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Vermont</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Wyoming</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fig4_data!$B$2:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2134448808"/>
+        <c:axId val="-2134464824"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="-2131684936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2130734072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2130734072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="0"/>
+                  <a:t>Voting pwoer</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2131684936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2134464824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="0"/>
+                  <a:t>Electoral</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="0" baseline="0"/>
+                  <a:t> Votes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000" b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2134448808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2134448808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2134464824"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
@@ -2306,6 +3999,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="144" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -2397,6 +4101,33 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8572500" cy="5829653"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pop_ev" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -2406,7 +4137,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="time_series" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="time_series" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solution" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4231,4 +5966,326 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>81896</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>81464</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>70597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>68806</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>66663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>63968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>54805</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>52031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>51136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>50977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>46410</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>46275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>45601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>42890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>42222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>41650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>38727</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>38601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>35877</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>35513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>34596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>33892</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>33203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>30901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>30618</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>